<commit_message>
Busqueda funcionarios por C_costo, registro ausentimso por hora
</commit_message>
<xml_diff>
--- a/assets/fun3.xlsx
+++ b/assets/fun3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Ausen2\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6949FAB-EE4F-45DA-B273-8EB2892EA215}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3FC3FF-F0E1-4915-9210-74DF5163CB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38520" yWindow="-5445" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcinarios Unicauca 2022" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="110">
   <si>
     <t>CODIGO</t>
   </si>
@@ -673,10 +673,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W24"/>
+  <dimension ref="A1:W23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1998,10 +1998,10 @@
         <v>23</v>
       </c>
       <c r="B22">
-        <v>1001086249</v>
+        <v>1001086250</v>
       </c>
       <c r="C22" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="D22" s="1">
         <v>44810</v>
@@ -2010,7 +2010,7 @@
         <v>40</v>
       </c>
       <c r="F22" t="s">
-        <v>101</v>
+        <v>30</v>
       </c>
       <c r="G22">
         <v>7200</v>
@@ -2022,7 +2022,7 @@
         <v>38</v>
       </c>
       <c r="J22">
-        <v>1143008</v>
+        <v>0</v>
       </c>
       <c r="K22" t="s">
         <v>44</v>
@@ -2055,7 +2055,7 @@
         <v>8316144</v>
       </c>
       <c r="W22" t="s">
-        <v>104</v>
+        <v>108</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.3">
@@ -2063,10 +2063,10 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>1001086250</v>
-      </c>
-      <c r="C23" t="s">
-        <v>107</v>
+        <v>1001086251</v>
+      </c>
+      <c r="C23">
+        <v>111</v>
       </c>
       <c r="D23" s="1">
         <v>44810</v>
@@ -2084,7 +2084,7 @@
         <v>1</v>
       </c>
       <c r="I23" t="s">
-        <v>38</v>
+        <v>109</v>
       </c>
       <c r="J23">
         <v>0</v>
@@ -2120,71 +2120,6 @@
         <v>8316144</v>
       </c>
       <c r="W23" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A24">
-        <v>23</v>
-      </c>
-      <c r="B24">
-        <v>1001086251</v>
-      </c>
-      <c r="C24">
-        <v>111</v>
-      </c>
-      <c r="D24" s="1">
-        <v>44810</v>
-      </c>
-      <c r="E24">
-        <v>40</v>
-      </c>
-      <c r="F24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24">
-        <v>7200</v>
-      </c>
-      <c r="H24">
-        <v>1</v>
-      </c>
-      <c r="I24" t="s">
-        <v>109</v>
-      </c>
-      <c r="J24">
-        <v>0</v>
-      </c>
-      <c r="K24" t="s">
-        <v>44</v>
-      </c>
-      <c r="L24" t="s">
-        <v>37</v>
-      </c>
-      <c r="M24">
-        <v>4</v>
-      </c>
-      <c r="N24">
-        <v>5006381</v>
-      </c>
-      <c r="O24" s="1">
-        <v>23114</v>
-      </c>
-      <c r="P24">
-        <v>59</v>
-      </c>
-      <c r="R24">
-        <v>29</v>
-      </c>
-      <c r="T24" t="s">
-        <v>106</v>
-      </c>
-      <c r="U24" t="s">
-        <v>96</v>
-      </c>
-      <c r="V24">
-        <v>8316144</v>
-      </c>
-      <c r="W24" t="s">
         <v>108</v>
       </c>
     </row>

</xml_diff>

<commit_message>
:ambulance: Se añade EPS y ARP a funcionarios.
Se modifica la base de datos y el registro de ausentismos.
</commit_message>
<xml_diff>
--- a/assets/fun3.xlsx
+++ b/assets/fun3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\Ausen2\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A3FC3FF-F0E1-4915-9210-74DF5163CB43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42698A22-4F34-423B-9B65-DDCA970476EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-33915" yWindow="-840" windowWidth="28800" windowHeight="15285" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Funcinarios Unicauca 2022" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="116">
   <si>
     <t>CODIGO</t>
   </si>
@@ -355,16 +355,48 @@
   </si>
   <si>
     <t>PROFESOR1 ASISTENTE</t>
+  </si>
+  <si>
+    <t>EPS</t>
+  </si>
+  <si>
+    <t>ARP</t>
+  </si>
+  <si>
+    <t>POSITIVA COMPAÑIA DE SEGUROS</t>
+  </si>
+  <si>
+    <t>NUEVA EPS</t>
+  </si>
+  <si>
+    <t>UNICAUCA UNID ESPECIAL SERVICIO DE SALUD</t>
+  </si>
+  <si>
+    <t>UNICAUCA UNID ESPECIAL SERVICIO DE SALUD11</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -390,9 +422,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -673,10 +708,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:W23"/>
+  <dimension ref="A1:Y23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="Y23" sqref="Y23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -685,80 +720,89 @@
     <col min="11" max="11" width="20.21875" customWidth="1"/>
     <col min="12" max="12" width="26.109375" customWidth="1"/>
     <col min="22" max="22" width="18.88671875" customWidth="1"/>
+    <col min="23" max="23" width="11.44140625" customWidth="1"/>
+    <col min="24" max="24" width="41.21875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="30.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:25" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="2" t="s">
         <v>4</v>
       </c>
+      <c r="X1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>111</v>
+      </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>920222</v>
       </c>
@@ -822,8 +866,14 @@
       <c r="W2" t="s">
         <v>102</v>
       </c>
+      <c r="X2" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>1920222</v>
       </c>
@@ -887,8 +937,14 @@
       <c r="W3" t="s">
         <v>102</v>
       </c>
+      <c r="X3" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>2520222</v>
       </c>
@@ -952,8 +1008,14 @@
       <c r="W4" t="s">
         <v>102</v>
       </c>
+      <c r="X4" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>34323720</v>
       </c>
@@ -1017,8 +1079,14 @@
       <c r="W5" t="s">
         <v>102</v>
       </c>
+      <c r="X5" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6520222</v>
       </c>
@@ -1082,8 +1150,14 @@
       <c r="W6" t="s">
         <v>102</v>
       </c>
+      <c r="X6" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6920223</v>
       </c>
@@ -1147,8 +1221,14 @@
       <c r="W7" t="s">
         <v>102</v>
       </c>
+      <c r="X7" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7020222</v>
       </c>
@@ -1212,8 +1292,14 @@
       <c r="W8" t="s">
         <v>102</v>
       </c>
+      <c r="X8" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>7320222</v>
       </c>
@@ -1277,8 +1363,14 @@
       <c r="W9" t="s">
         <v>102</v>
       </c>
+      <c r="X9" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>76319254</v>
       </c>
@@ -1342,8 +1434,14 @@
       <c r="W10" t="s">
         <v>102</v>
       </c>
+      <c r="X10" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>8220222</v>
       </c>
@@ -1407,8 +1505,14 @@
       <c r="W11" t="s">
         <v>102</v>
       </c>
+      <c r="X11" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>8320222</v>
       </c>
@@ -1472,8 +1576,14 @@
       <c r="W12" t="s">
         <v>102</v>
       </c>
+      <c r="X12" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8520222</v>
       </c>
@@ -1537,8 +1647,14 @@
       <c r="W13" t="s">
         <v>102</v>
       </c>
+      <c r="X13" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8620222</v>
       </c>
@@ -1602,8 +1718,14 @@
       <c r="W14" t="s">
         <v>102</v>
       </c>
+      <c r="X14" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>9020223</v>
       </c>
@@ -1667,8 +1789,14 @@
       <c r="W15" t="s">
         <v>102</v>
       </c>
+      <c r="X15" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>10120222</v>
       </c>
@@ -1732,8 +1860,14 @@
       <c r="W16" t="s">
         <v>102</v>
       </c>
+      <c r="X16" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>10520222</v>
       </c>
@@ -1797,8 +1931,14 @@
       <c r="W17" t="s">
         <v>102</v>
       </c>
+      <c r="X17" t="s">
+        <v>113</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>23</v>
       </c>
@@ -1862,8 +2002,14 @@
       <c r="W18" t="s">
         <v>102</v>
       </c>
+      <c r="X18" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>23</v>
       </c>
@@ -1927,8 +2073,14 @@
       <c r="W20" t="s">
         <v>103</v>
       </c>
+      <c r="X20" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>23</v>
       </c>
@@ -1992,8 +2144,14 @@
       <c r="W21" t="s">
         <v>104</v>
       </c>
+      <c r="X21" t="s">
+        <v>114</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>23</v>
       </c>
@@ -2057,8 +2215,14 @@
       <c r="W22" t="s">
         <v>108</v>
       </c>
+      <c r="X22" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>112</v>
+      </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>23</v>
       </c>
@@ -2122,8 +2286,13 @@
       <c r="W23" t="s">
         <v>108</v>
       </c>
+      <c r="X23" t="s">
+        <v>114</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>